<commit_message>
2.12.9 update doc (xls for scale and offset) + fields srxl/ibus
</commit_message>
<xml_diff>
--- a/doc/Calculate_scale_and_offset.xlsx
+++ b/doc/Calculate_scale_and_offset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Values on handset (with scale=1 and offset =0)</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>&lt;= Do not change</t>
+  </si>
+  <si>
+    <t>Important: values filled in the yellow cells should be in the same units as the units used internally by oXs (e.g. milliVolt or milliAmpere)</t>
+  </si>
+  <si>
+    <t>oXs will transmit to the handset =&gt;</t>
+  </si>
+  <si>
+    <t>so when oXs will measure e.g. =&gt;</t>
+  </si>
+  <si>
+    <t>mv</t>
+  </si>
+  <si>
+    <t>Please note that the units on the handset can be different (e.g. A instead of mA)</t>
   </si>
 </sst>
 </file>
@@ -198,9 +213,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:trendline>
             <c:trendlineType val="linear"/>
             <c:dispEq val="1"/>
@@ -216,13 +228,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1670</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -234,35 +246,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124980608"/>
-        <c:axId val="100674944"/>
+        <c:axId val="36215040"/>
+        <c:axId val="40060800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124980608"/>
+        <c:axId val="36215040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100674944"/>
+        <c:crossAx val="40060800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100674944"/>
+        <c:axId val="40060800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -270,7 +282,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124980608"/>
+        <c:crossAx val="36215040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -283,7 +295,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -293,16 +305,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -609,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -630,18 +642,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1">
-        <v>140</v>
+        <v>18000</v>
       </c>
       <c r="D5" s="1">
-        <v>160</v>
+        <v>40000</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -652,13 +669,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>10</v>
+        <v>1670</v>
       </c>
       <c r="C6" s="1">
-        <v>20</v>
+        <v>2150</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>2700</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -670,15 +687,15 @@
       </c>
       <c r="B8">
         <f>TREND($B$5:$D$5,$B$6:$D$6,B6)</f>
-        <v>107.5</v>
+        <v>-138.63533693061618</v>
       </c>
       <c r="C8">
         <f>TREND($B$5:$D$5,$B$6:$D$6,C6)</f>
-        <v>135</v>
+        <v>18465.626176433681</v>
       </c>
       <c r="D8">
         <f>TREND($B$5:$D$5,$B$6:$D$6,D6)</f>
-        <v>162.5</v>
+        <v>39783.009160496935</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -695,7 +712,7 @@
       </c>
       <c r="B13" s="2">
         <f>(D8-B8)/(D6-B6)</f>
-        <v>2.75</v>
+        <v>38.758878152842286</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1">
@@ -704,7 +721,32 @@
       </c>
       <c r="B14" s="3">
         <f>-B8+B6*B13</f>
-        <v>-80</v>
+        <v>64865.961852177235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2700</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <f>B17*B13-B14</f>
+        <v>39783.009160496935</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>